<commit_message>
Added bed plan data
</commit_message>
<xml_diff>
--- a/Data/bed_plan.xlsx
+++ b/Data/bed_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliverlambson/GitHub/ISMM/CUH_covid_tactical_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661FB956-196E-CF4C-BFD4-45AC89DB64DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F670AC-93B7-FC44-A91B-6C3D3284FEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" activeTab="1" xr2:uid="{893A1198-EF4A-374B-878D-BB99CEBFF327}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{893A1198-EF4A-374B-878D-BB99CEBFF327}"/>
   </bookViews>
   <sheets>
     <sheet name="v14" sheetId="1" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912AF5BF-08E4-B948-82EF-43F43AA8190D}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2909,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF8E4E8-E588-764E-88ED-B4B85744FD50}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>